<commit_message>
Updating PLR/Probabilities sheets to include more 2AP scenarios
</commit_message>
<xml_diff>
--- a/input_files/probabilities.xlsx
+++ b/input_files/probabilities.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T\PycharmProjects\find-max-ssp\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56EC028-C795-4E11-B4C7-E5972D7B8DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA109A2-D3D1-4235-A130-7314A364657E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F01DBDD6-AB74-4653-B50F-8191F1E572B0}"/>
+    <workbookView xWindow="16371" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{F01DBDD6-AB74-4653-B50F-8191F1E572B0}"/>
   </bookViews>
   <sheets>
     <sheet name="probabilities" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -512,7 +525,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -573,8 +588,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BC94697F-88AC-4CD6-84E3-57F8BB03B88A}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
-  <autoFilter ref="A1:B19" xr:uid="{BC94697F-88AC-4CD6-84E3-57F8BB03B88A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BC94697F-88AC-4CD6-84E3-57F8BB03B88A}" name="Table1" displayName="Table1" ref="A1:B28" totalsRowShown="0">
+  <autoFilter ref="A1:B28" xr:uid="{BC94697F-88AC-4CD6-84E3-57F8BB03B88A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D584EBA0-62D9-429A-B60D-BA5FF0C8B31A}" name="Scenario_Name"/>
     <tableColumn id="2" xr3:uid="{61737258-99F9-4618-97AA-5D1129355674}" name="Probability"/>
@@ -900,19 +915,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81390177-B1FB-45E1-8E1C-FBCA0926D8C5}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.19921875" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="1" max="1" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -920,148 +935,214 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="1">
         <v>12345</v>
       </c>
-      <c r="B2">
-        <v>0.155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="B2" s="2">
+        <v>0.13139999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
+        <v>2345</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4.9299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
+        <v>1345</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
+        <v>1245</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.9299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>1235</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.3100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
         <v>1234</v>
       </c>
-      <c r="B3">
-        <v>5.8099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1235</v>
-      </c>
-      <c r="B4">
-        <v>1.55E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>2345</v>
-      </c>
-      <c r="B5">
-        <v>5.8099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>1345</v>
-      </c>
-      <c r="B6">
-        <v>1.55E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>1245</v>
-      </c>
-      <c r="B7">
-        <v>5.8099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8">
+      <c r="B7" s="2">
+        <v>4.9299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="1">
         <v>123</v>
       </c>
-      <c r="B8">
-        <v>1.49E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9">
+      <c r="B8" s="2">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
         <v>124</v>
       </c>
-      <c r="B9">
-        <v>6.9699999999999998E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10">
+      <c r="B9" s="2">
+        <v>5.91E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
         <v>125</v>
       </c>
-      <c r="B10">
-        <v>1.49E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11">
+      <c r="B10" s="2">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="1">
         <v>134</v>
       </c>
-      <c r="B11">
-        <v>1.49E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12">
+      <c r="B11" s="2">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="1">
         <v>135</v>
       </c>
-      <c r="B12">
-        <v>3.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13">
+      <c r="B12" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" s="1">
         <v>145</v>
       </c>
-      <c r="B13">
-        <v>1.49E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14">
+      <c r="B13" s="2">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" s="1">
         <v>234</v>
       </c>
-      <c r="B14">
-        <v>6.9699999999999998E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="B14" s="2">
+        <v>5.91E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" s="1">
         <v>235</v>
       </c>
-      <c r="B15">
-        <v>1.49E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16">
+      <c r="B15" s="2">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" s="1">
         <v>245</v>
       </c>
-      <c r="B16">
-        <v>6.9699999999999998E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17">
+      <c r="B16" s="2">
+        <v>5.91E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1">
         <v>345</v>
       </c>
-      <c r="B17">
-        <v>1.49E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18">
+      <c r="B17" s="2">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="1">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3.3799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="1">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="1">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3.3799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="1">
         <v>24</v>
       </c>
-      <c r="B18">
-        <v>0.314</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+      <c r="B22" s="2">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="1">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3.3799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="1">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3.3799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19">
-        <v>2.3699999999999999E-2</v>
+      <c r="B26" s="2">
+        <v>2.01E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2">
+        <v>1.0003000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>